<commit_message>
Updated excel file for part1
</commit_message>
<xml_diff>
--- a/ClueMap.xlsx
+++ b/ClueMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcassata/Documents/GitHub/clue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:19_{4EABB148-8E73-A54B-91A4-A5A483F7C00C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BCC1287B-6086-6049-BA7A-F465308CD699}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14480" xr2:uid="{10111C03-15FD-B84E-A992-C235F73A671F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{10111C03-15FD-B84E-A992-C235F73A671F}"/>
   </bookViews>
   <sheets>
     <sheet name="ClueMap" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +162,42 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCF7BEF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -175,18 +211,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCF7BEF"/>
+      <color rgb="FFFF9EED"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -497,8 +545,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2382C08F-1113-E441-9669-FF0235B4F9DF}">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -519,7 +567,7 @@
       <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -907,7 +955,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -928,7 +976,7 @@
       <c r="G6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="10" t="s">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -943,13 +991,13 @@
       <c r="L6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="P6" s="2" t="s">
@@ -1029,7 +1077,7 @@
       <c r="N7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -1079,7 +1127,7 @@
       <c r="D8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -1115,7 +1163,7 @@
       <c r="P8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="R8" s="2" t="s">
@@ -1322,7 +1370,7 @@
       <c r="E11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1379,7 +1427,7 @@
       <c r="X11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="Y11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="Z11">
@@ -1402,7 +1450,7 @@
       <c r="E12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1432,7 +1480,7 @@
       <c r="O12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q12" s="2" t="s">
@@ -1512,7 +1560,7 @@
       <c r="O13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="Q13" s="2" t="s">
@@ -1547,7 +1595,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1690,7 +1738,7 @@
       <c r="U15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V15" s="2" t="s">
+      <c r="V15" s="9" t="s">
         <v>24</v>
       </c>
       <c r="W15" s="2" t="s">
@@ -1770,7 +1818,7 @@
       <c r="U16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="V16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="W16" s="1" t="s">
@@ -1802,7 +1850,7 @@
       <c r="E17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="10" t="s">
         <v>21</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -1992,7 +2040,7 @@
       <c r="O19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="P19" s="5" t="s">
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="s">
@@ -2027,7 +2075,7 @@
       </c>
     </row>
     <row r="20" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2084,7 +2132,7 @@
       <c r="S20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="T20" s="2" t="s">
+      <c r="T20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="U20" s="2" t="s">
@@ -2107,7 +2155,7 @@
       </c>
     </row>
     <row r="21" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2229,10 +2277,10 @@
       <c r="N22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="O22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="P22" s="10" t="s">
         <v>0</v>
       </c>
       <c r="Q22" s="1" t="s">
@@ -2315,7 +2363,7 @@
       <c r="P23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="Q23" s="7" t="s">
         <v>0</v>
       </c>
       <c r="R23" s="4" t="s">
@@ -2339,7 +2387,7 @@
       <c r="X23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Y23" s="2" t="s">
+      <c r="Y23" s="6" t="s">
         <v>3</v>
       </c>
       <c r="Z23">

</xml_diff>